<commit_message>
Update on performance new table  view on mortages pdf function roles udpate data filled docker working
</commit_message>
<xml_diff>
--- a/AMIGO UI.xlsx
+++ b/AMIGO UI.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/073c81f67e416fdc/Desktop/‎/GPGLOBAL/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/073c81f67e416fdc/Desktop/‎/GPGLOBAL/loan-service-system-main-2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1268" documentId="8_{A29C76CF-9D70-4178-9CA6-F30F45099062}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BF900918-A47F-4178-A832-A699C588E307}"/>
+  <xr:revisionPtr revIDLastSave="1270" documentId="8_{A29C76CF-9D70-4178-9CA6-F30F45099062}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F1B780B0-A3D3-48A3-A7AA-BC7E575DB83E}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="2" xr2:uid="{217603A9-211F-43B7-8100-070EC3968530}"/>
   </bookViews>
@@ -1267,17 +1267,37 @@
     <xf numFmtId="10" fontId="0" fillId="17" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="14" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1291,20 +1311,6 @@
     <xf numFmtId="0" fontId="11" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
@@ -1314,12 +1320,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="11" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -3631,8 +3631,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{987F612E-7D92-4C38-B3E4-594A22572CC7}">
   <dimension ref="A2:X36"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:H11"/>
+    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="H35" sqref="A21:H35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3659,62 +3659,62 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="F2" s="97" t="s">
+      <c r="F2" s="79" t="s">
         <v>52</v>
       </c>
-      <c r="G2" s="81"/>
+      <c r="G2" s="78"/>
       <c r="H2" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="O2" s="97" t="s">
+      <c r="O2" s="79" t="s">
         <v>52</v>
       </c>
-      <c r="P2" s="81"/>
+      <c r="P2" s="78"/>
       <c r="Q2" s="7" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F3" s="98" t="s">
+      <c r="F3" s="80" t="s">
         <v>54</v>
       </c>
-      <c r="G3" s="80"/>
-      <c r="H3" s="81"/>
-      <c r="O3" s="98" t="s">
+      <c r="G3" s="81"/>
+      <c r="H3" s="78"/>
+      <c r="O3" s="80" t="s">
         <v>54</v>
       </c>
-      <c r="P3" s="80"/>
-      <c r="Q3" s="81"/>
+      <c r="P3" s="81"/>
+      <c r="Q3" s="78"/>
     </row>
     <row r="4" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F4" s="87" t="s">
+      <c r="F4" s="77" t="s">
         <v>55</v>
       </c>
-      <c r="G4" s="81"/>
+      <c r="G4" s="78"/>
       <c r="H4" s="8">
         <f>+'Corporate View '!F8</f>
         <v>11693.534625</v>
       </c>
-      <c r="O4" s="87" t="s">
+      <c r="O4" s="77" t="s">
         <v>55</v>
       </c>
-      <c r="P4" s="81"/>
+      <c r="P4" s="78"/>
       <c r="Q4" s="8">
         <v>1000</v>
       </c>
     </row>
     <row r="5" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F5" s="87" t="s">
+      <c r="F5" s="77" t="s">
         <v>56</v>
       </c>
-      <c r="G5" s="81"/>
+      <c r="G5" s="78"/>
       <c r="H5" s="9">
         <v>0</v>
       </c>
-      <c r="O5" s="87" t="s">
+      <c r="O5" s="77" t="s">
         <v>56</v>
       </c>
-      <c r="P5" s="81"/>
+      <c r="P5" s="78"/>
       <c r="Q5" s="9">
         <v>0</v>
       </c>
@@ -3724,128 +3724,128 @@
       </c>
     </row>
     <row r="6" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F6" s="87" t="s">
+      <c r="F6" s="77" t="s">
         <v>57</v>
       </c>
-      <c r="G6" s="81"/>
+      <c r="G6" s="78"/>
       <c r="H6" s="10">
         <f>H5*H4</f>
         <v>0</v>
       </c>
-      <c r="O6" s="87" t="s">
+      <c r="O6" s="77" t="s">
         <v>57</v>
       </c>
-      <c r="P6" s="81"/>
+      <c r="P6" s="78"/>
       <c r="Q6" s="10">
         <f>Q5*Q4</f>
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F7" s="87" t="s">
+      <c r="F7" s="77" t="s">
         <v>58</v>
       </c>
-      <c r="G7" s="81"/>
+      <c r="G7" s="78"/>
       <c r="H7" s="10">
         <f>H4-H6</f>
         <v>11693.534625</v>
       </c>
-      <c r="O7" s="87" t="s">
+      <c r="O7" s="77" t="s">
         <v>58</v>
       </c>
-      <c r="P7" s="81"/>
+      <c r="P7" s="78"/>
       <c r="Q7" s="10">
         <f>Q4-Q6</f>
         <v>1000</v>
       </c>
     </row>
     <row r="8" spans="1:24" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F8" s="87" t="s">
+      <c r="F8" s="77" t="s">
         <v>59</v>
       </c>
-      <c r="G8" s="81"/>
+      <c r="G8" s="78"/>
       <c r="H8" s="11">
         <f>+'Corporate View '!H3</f>
         <v>0.34194805194805195</v>
       </c>
-      <c r="O8" s="87" t="s">
+      <c r="O8" s="77" t="s">
         <v>59</v>
       </c>
-      <c r="P8" s="81"/>
+      <c r="P8" s="78"/>
       <c r="Q8" s="11">
         <v>0.35</v>
       </c>
     </row>
     <row r="9" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F9" s="87" t="s">
+      <c r="F9" s="77" t="s">
         <v>60</v>
       </c>
-      <c r="G9" s="81"/>
+      <c r="G9" s="78"/>
       <c r="H9" s="12">
         <v>1</v>
       </c>
-      <c r="O9" s="87" t="s">
+      <c r="O9" s="77" t="s">
         <v>60</v>
       </c>
-      <c r="P9" s="81"/>
+      <c r="P9" s="78"/>
       <c r="Q9" s="12">
         <v>1</v>
       </c>
       <c r="X9" s="71"/>
     </row>
     <row r="10" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="F10" s="87" t="s">
+      <c r="F10" s="77" t="s">
         <v>61</v>
       </c>
-      <c r="G10" s="81"/>
+      <c r="G10" s="78"/>
       <c r="H10" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="O10" s="87" t="s">
+      <c r="O10" s="77" t="s">
         <v>61</v>
       </c>
-      <c r="P10" s="81"/>
+      <c r="P10" s="78"/>
       <c r="Q10" s="12" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="11" spans="1:24" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F11" s="88" t="s">
+      <c r="F11" s="83" t="s">
         <v>63</v>
       </c>
-      <c r="G11" s="89"/>
+      <c r="G11" s="84"/>
       <c r="H11" s="13">
         <v>45678</v>
       </c>
-      <c r="O11" s="88" t="s">
+      <c r="O11" s="83" t="s">
         <v>63</v>
       </c>
-      <c r="P11" s="89"/>
+      <c r="P11" s="84"/>
       <c r="Q11" s="13">
         <v>45689</v>
       </c>
     </row>
     <row r="12" spans="1:24" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F12" s="90"/>
-      <c r="G12" s="80"/>
+      <c r="F12" s="85"/>
+      <c r="G12" s="81"/>
       <c r="H12" s="14"/>
-      <c r="O12" s="90"/>
-      <c r="P12" s="80"/>
+      <c r="O12" s="85"/>
+      <c r="P12" s="81"/>
       <c r="Q12" s="14"/>
     </row>
     <row r="13" spans="1:24" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F13" s="91" t="s">
+      <c r="F13" s="86" t="s">
         <v>64</v>
       </c>
-      <c r="G13" s="92"/>
+      <c r="G13" s="87"/>
       <c r="H13" s="15">
         <f>H8/12</f>
         <v>2.8495670995670994E-2</v>
       </c>
-      <c r="O13" s="91" t="s">
+      <c r="O13" s="86" t="s">
         <v>64</v>
       </c>
-      <c r="P13" s="92"/>
+      <c r="P13" s="87"/>
       <c r="Q13" s="15">
         <f>Q8/12</f>
         <v>2.9166666666666664E-2</v>
@@ -3856,10 +3856,10 @@
       <c r="E14" t="s">
         <v>65</v>
       </c>
-      <c r="F14" s="93" t="s">
+      <c r="F14" s="95" t="s">
         <v>66</v>
       </c>
-      <c r="G14" s="81"/>
+      <c r="G14" s="78"/>
       <c r="H14" s="16">
         <f>ROUND(-PMT(H13,C19,H7),2)</f>
         <v>1164.23</v>
@@ -3867,10 +3867,10 @@
       <c r="N14" t="s">
         <v>65</v>
       </c>
-      <c r="O14" s="93" t="s">
+      <c r="O14" s="95" t="s">
         <v>66</v>
       </c>
-      <c r="P14" s="81"/>
+      <c r="P14" s="78"/>
       <c r="Q14" s="16">
         <f>ROUND(-PMT(Q13,L19,Q7),2)</f>
         <v>99.96</v>
@@ -3880,10 +3880,10 @@
       <c r="E15" t="s">
         <v>67</v>
       </c>
-      <c r="F15" s="93" t="s">
+      <c r="F15" s="95" t="s">
         <v>68</v>
       </c>
-      <c r="G15" s="81"/>
+      <c r="G15" s="78"/>
       <c r="H15" s="17">
         <f>C19</f>
         <v>12</v>
@@ -3891,10 +3891,10 @@
       <c r="N15" t="s">
         <v>67</v>
       </c>
-      <c r="O15" s="93" t="s">
+      <c r="O15" s="95" t="s">
         <v>68</v>
       </c>
-      <c r="P15" s="81"/>
+      <c r="P15" s="78"/>
       <c r="Q15" s="17">
         <f>L19</f>
         <v>12</v>
@@ -3908,10 +3908,10 @@
       <c r="E16" s="22" t="s">
         <v>69</v>
       </c>
-      <c r="F16" s="93" t="s">
+      <c r="F16" s="95" t="s">
         <v>70</v>
       </c>
-      <c r="G16" s="81"/>
+      <c r="G16" s="78"/>
       <c r="H16" s="16">
         <f>SUM(F24:F49)</f>
         <v>2277.2599999999998</v>
@@ -3923,10 +3923,10 @@
       <c r="N16" s="22" t="s">
         <v>69</v>
       </c>
-      <c r="O16" s="93" t="s">
+      <c r="O16" s="95" t="s">
         <v>70</v>
       </c>
-      <c r="P16" s="81"/>
+      <c r="P16" s="78"/>
       <c r="Q16" s="16">
         <f>SUM(O24:O49)</f>
         <v>28.5</v>
@@ -3934,10 +3934,10 @@
       <c r="X16" s="16"/>
     </row>
     <row r="17" spans="1:21" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A17" s="94" t="s">
+      <c r="A17" s="96" t="s">
         <v>71</v>
       </c>
-      <c r="B17" s="95"/>
+      <c r="B17" s="97"/>
       <c r="C17" s="23">
         <f t="array" ref="C17">INDEX({1;2;4;6;12;24;26;52},MATCH($H$10,$E$13:$E$20,0))</f>
         <v>12</v>
@@ -3946,17 +3946,17 @@
       <c r="E17" s="25" t="s">
         <v>62</v>
       </c>
-      <c r="F17" s="96" t="s">
+      <c r="F17" s="98" t="s">
         <v>72</v>
       </c>
-      <c r="G17" s="95"/>
+      <c r="G17" s="97"/>
       <c r="H17" s="26" t="s">
         <v>73</v>
       </c>
-      <c r="J17" s="94" t="s">
+      <c r="J17" s="96" t="s">
         <v>71</v>
       </c>
-      <c r="K17" s="95"/>
+      <c r="K17" s="97"/>
       <c r="L17" s="23">
         <f t="array" ref="L17">INDEX({1;2;4;6;12;24;26;52},MATCH($H$10,$E$13:$E$20,0))</f>
         <v>12</v>
@@ -3965,19 +3965,19 @@
       <c r="N17" s="25" t="s">
         <v>62</v>
       </c>
-      <c r="O17" s="96" t="s">
+      <c r="O17" s="98" t="s">
         <v>72</v>
       </c>
-      <c r="P17" s="95"/>
+      <c r="P17" s="97"/>
       <c r="Q17" s="26" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="18" spans="1:21" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A18" s="77" t="s">
+      <c r="A18" s="82" t="s">
         <v>74</v>
       </c>
-      <c r="B18" s="77"/>
+      <c r="B18" s="82"/>
       <c r="C18" s="23">
         <f>12/$C$17</f>
         <v>1</v>
@@ -3989,10 +3989,10 @@
       <c r="F18" s="27"/>
       <c r="G18" s="28"/>
       <c r="H18" s="29"/>
-      <c r="J18" s="77" t="s">
+      <c r="J18" s="82" t="s">
         <v>74</v>
       </c>
-      <c r="K18" s="77"/>
+      <c r="K18" s="82"/>
       <c r="L18" s="23">
         <f>12/$C$17</f>
         <v>1</v>
@@ -4006,10 +4006,10 @@
       <c r="Q18" s="29"/>
     </row>
     <row r="19" spans="1:21" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A19" s="77" t="s">
+      <c r="A19" s="82" t="s">
         <v>75</v>
       </c>
-      <c r="B19" s="77"/>
+      <c r="B19" s="82"/>
       <c r="C19" s="23">
         <f>$H$9*$C$17</f>
         <v>12</v>
@@ -4021,10 +4021,10 @@
       <c r="F19" s="27"/>
       <c r="G19" s="28"/>
       <c r="H19" s="29"/>
-      <c r="J19" s="77" t="s">
+      <c r="J19" s="82" t="s">
         <v>75</v>
       </c>
-      <c r="K19" s="77"/>
+      <c r="K19" s="82"/>
       <c r="L19" s="23">
         <f>$H$9*$C$17</f>
         <v>12</v>
@@ -4038,10 +4038,10 @@
       <c r="Q19" s="29"/>
     </row>
     <row r="20" spans="1:21" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A20" s="78" t="s">
+      <c r="A20" s="88" t="s">
         <v>77</v>
       </c>
-      <c r="B20" s="78"/>
+      <c r="B20" s="88"/>
       <c r="C20" s="30" t="b">
         <f>(H17="En")</f>
         <v>1</v>
@@ -4053,10 +4053,10 @@
       <c r="F20" s="27"/>
       <c r="G20" s="28"/>
       <c r="H20" s="29"/>
-      <c r="J20" s="78" t="s">
+      <c r="J20" s="88" t="s">
         <v>77</v>
       </c>
-      <c r="K20" s="78"/>
+      <c r="K20" s="88"/>
       <c r="L20" s="30" t="b">
         <f>(Q17="En")</f>
         <v>1</v>
@@ -4070,71 +4070,71 @@
       <c r="Q20" s="29"/>
     </row>
     <row r="21" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A21" s="79" t="s">
+      <c r="A21" s="89" t="s">
         <v>79</v>
       </c>
-      <c r="B21" s="80"/>
-      <c r="C21" s="80"/>
-      <c r="D21" s="80"/>
-      <c r="E21" s="80"/>
-      <c r="F21" s="80"/>
-      <c r="G21" s="80"/>
-      <c r="H21" s="81"/>
-      <c r="J21" s="79" t="s">
+      <c r="B21" s="81"/>
+      <c r="C21" s="81"/>
+      <c r="D21" s="81"/>
+      <c r="E21" s="81"/>
+      <c r="F21" s="81"/>
+      <c r="G21" s="81"/>
+      <c r="H21" s="78"/>
+      <c r="J21" s="89" t="s">
         <v>79</v>
       </c>
-      <c r="K21" s="80"/>
-      <c r="L21" s="80"/>
-      <c r="M21" s="80"/>
-      <c r="N21" s="80"/>
-      <c r="O21" s="80"/>
-      <c r="P21" s="80"/>
-      <c r="Q21" s="81"/>
+      <c r="K21" s="81"/>
+      <c r="L21" s="81"/>
+      <c r="M21" s="81"/>
+      <c r="N21" s="81"/>
+      <c r="O21" s="81"/>
+      <c r="P21" s="81"/>
+      <c r="Q21" s="78"/>
     </row>
     <row r="22" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A22" s="82" t="s">
+      <c r="A22" s="90" t="s">
         <v>80</v>
       </c>
-      <c r="B22" s="82" t="s">
+      <c r="B22" s="90" t="s">
         <v>81</v>
       </c>
-      <c r="C22" s="84" t="s">
+      <c r="C22" s="92" t="s">
         <v>82</v>
       </c>
-      <c r="D22" s="85" t="s">
+      <c r="D22" s="93" t="s">
         <v>83</v>
       </c>
-      <c r="E22" s="86" t="s">
+      <c r="E22" s="94" t="s">
         <v>84</v>
       </c>
-      <c r="F22" s="85" t="s">
+      <c r="F22" s="93" t="s">
         <v>85</v>
       </c>
-      <c r="G22" s="85" t="s">
+      <c r="G22" s="93" t="s">
         <v>86</v>
       </c>
       <c r="H22" s="32" t="s">
         <v>87</v>
       </c>
-      <c r="J22" s="82" t="s">
+      <c r="J22" s="90" t="s">
         <v>80</v>
       </c>
-      <c r="K22" s="82" t="s">
+      <c r="K22" s="90" t="s">
         <v>81</v>
       </c>
-      <c r="L22" s="84" t="s">
+      <c r="L22" s="92" t="s">
         <v>82</v>
       </c>
-      <c r="M22" s="85" t="s">
+      <c r="M22" s="93" t="s">
         <v>83</v>
       </c>
-      <c r="N22" s="86" t="s">
+      <c r="N22" s="94" t="s">
         <v>84</v>
       </c>
-      <c r="O22" s="85" t="s">
+      <c r="O22" s="93" t="s">
         <v>85</v>
       </c>
-      <c r="P22" s="85" t="s">
+      <c r="P22" s="93" t="s">
         <v>86</v>
       </c>
       <c r="Q22" s="32" t="s">
@@ -4142,24 +4142,24 @@
       </c>
     </row>
     <row r="23" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A23" s="83"/>
-      <c r="B23" s="83"/>
-      <c r="C23" s="83"/>
-      <c r="D23" s="83"/>
-      <c r="E23" s="83"/>
-      <c r="F23" s="83"/>
-      <c r="G23" s="83"/>
+      <c r="A23" s="91"/>
+      <c r="B23" s="91"/>
+      <c r="C23" s="91"/>
+      <c r="D23" s="91"/>
+      <c r="E23" s="91"/>
+      <c r="F23" s="91"/>
+      <c r="G23" s="91"/>
       <c r="H23" s="33">
         <f>H7</f>
         <v>11693.534625</v>
       </c>
-      <c r="J23" s="83"/>
-      <c r="K23" s="83"/>
-      <c r="L23" s="83"/>
-      <c r="M23" s="83"/>
-      <c r="N23" s="83"/>
-      <c r="O23" s="83"/>
-      <c r="P23" s="83"/>
+      <c r="J23" s="91"/>
+      <c r="K23" s="91"/>
+      <c r="L23" s="91"/>
+      <c r="M23" s="91"/>
+      <c r="N23" s="91"/>
+      <c r="O23" s="91"/>
+      <c r="P23" s="91"/>
       <c r="Q23" s="33">
         <f>Q7</f>
         <v>1000</v>
@@ -4990,19 +4990,33 @@
     </row>
   </sheetData>
   <mergeCells count="56">
-    <mergeCell ref="F7:G7"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="F3:H3"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="F5:G5"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="F8:G8"/>
-    <mergeCell ref="F9:G9"/>
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="F11:G11"/>
-    <mergeCell ref="F12:G12"/>
-    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="J19:K19"/>
+    <mergeCell ref="J20:K20"/>
+    <mergeCell ref="J21:Q21"/>
+    <mergeCell ref="J22:J23"/>
+    <mergeCell ref="K22:K23"/>
+    <mergeCell ref="L22:L23"/>
+    <mergeCell ref="M22:M23"/>
+    <mergeCell ref="N22:N23"/>
+    <mergeCell ref="O22:O23"/>
+    <mergeCell ref="P22:P23"/>
+    <mergeCell ref="J18:K18"/>
+    <mergeCell ref="O8:P8"/>
+    <mergeCell ref="O9:P9"/>
+    <mergeCell ref="O10:P10"/>
+    <mergeCell ref="O11:P11"/>
+    <mergeCell ref="O12:P12"/>
+    <mergeCell ref="O13:P13"/>
+    <mergeCell ref="O14:P14"/>
+    <mergeCell ref="O15:P15"/>
+    <mergeCell ref="O16:P16"/>
+    <mergeCell ref="J17:K17"/>
+    <mergeCell ref="O17:P17"/>
+    <mergeCell ref="O2:P2"/>
+    <mergeCell ref="O3:Q3"/>
+    <mergeCell ref="O4:P4"/>
+    <mergeCell ref="O5:P5"/>
+    <mergeCell ref="O6:P6"/>
     <mergeCell ref="O7:P7"/>
     <mergeCell ref="A19:B19"/>
     <mergeCell ref="A20:B20"/>
@@ -5019,33 +5033,19 @@
     <mergeCell ref="F16:G16"/>
     <mergeCell ref="A17:B17"/>
     <mergeCell ref="F17:G17"/>
-    <mergeCell ref="O2:P2"/>
-    <mergeCell ref="O3:Q3"/>
-    <mergeCell ref="O4:P4"/>
-    <mergeCell ref="O5:P5"/>
-    <mergeCell ref="O6:P6"/>
-    <mergeCell ref="J18:K18"/>
-    <mergeCell ref="O8:P8"/>
-    <mergeCell ref="O9:P9"/>
-    <mergeCell ref="O10:P10"/>
-    <mergeCell ref="O11:P11"/>
-    <mergeCell ref="O12:P12"/>
-    <mergeCell ref="O13:P13"/>
-    <mergeCell ref="O14:P14"/>
-    <mergeCell ref="O15:P15"/>
-    <mergeCell ref="O16:P16"/>
-    <mergeCell ref="J17:K17"/>
-    <mergeCell ref="O17:P17"/>
-    <mergeCell ref="J19:K19"/>
-    <mergeCell ref="J20:K20"/>
-    <mergeCell ref="J21:Q21"/>
-    <mergeCell ref="J22:J23"/>
-    <mergeCell ref="K22:K23"/>
-    <mergeCell ref="L22:L23"/>
-    <mergeCell ref="M22:M23"/>
-    <mergeCell ref="N22:N23"/>
-    <mergeCell ref="O22:O23"/>
-    <mergeCell ref="P22:P23"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="F9:G9"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="F3:H3"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="F6:G6"/>
   </mergeCells>
   <dataValidations disablePrompts="1" count="2">
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="H10 Q10" xr:uid="{5103491A-35BA-4E84-BBF9-5795A8DF4D3F}">

</xml_diff>